<commit_message>
renamed opaque to intransparent, improved evaluation, added back button to ExperimentController, disabled searchField when layer is deactivated
</commit_message>
<xml_diff>
--- a/ui/Evaluation Filter/Protokolle.xlsx
+++ b/ui/Evaluation Filter/Protokolle.xlsx
@@ -2,18 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefan/Documents/Code/Javascript/Getaviz/ui/Evaluation Filter/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6720" yWindow="0" windowWidth="22080" windowHeight="18000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26480" windowHeight="21600" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Testdurchlauf (David)" sheetId="2" r:id="rId1"/>
     <sheet name="Testdurchlauf (Pascal)" sheetId="1" r:id="rId2"/>
+    <sheet name="Template" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="75">
   <si>
     <t>Protokoll RedPill</t>
   </si>
@@ -235,6 +236,24 @@
   </si>
   <si>
     <t>hinweistimer</t>
+  </si>
+  <si>
+    <t>TODO:</t>
+  </si>
+  <si>
+    <t>Maybe:</t>
+  </si>
+  <si>
+    <t>0. Vorbereitung</t>
+  </si>
+  <si>
+    <t>Fragebögen öffnen, Getaviz zurücksetzen, User Guide öffnen, Screenrecording vorbereiten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uhrzeit: </t>
+  </si>
+  <si>
+    <t>10. Verabschiedung</t>
   </si>
 </sst>
 </file>
@@ -300,19 +319,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -591,10 +622,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H40"/>
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -604,53 +636,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="5"/>
+      <c r="D1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="2">
         <v>0.54722222222222217</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -696,10 +728,10 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="2">
         <v>0.55208333333333337</v>
       </c>
     </row>
@@ -791,44 +823,54 @@
         <v>46</v>
       </c>
     </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>41</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -851,10 +893,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H39"/>
+  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -864,53 +907,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="5"/>
+      <c r="D1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="2">
         <v>0.58819444444444446</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -959,10 +1002,10 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="5"/>
+      <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1045,62 +1088,72 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1119,4 +1172,216 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1:H28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="137" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="D1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="9"/>
+      <c r="B5" s="8"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId3"/>
+    <hyperlink ref="D1" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added final state after evaluation (use this commit to reference prototype)
</commit_message>
<xml_diff>
--- a/ui/Evaluation Filter/Protokolle.xlsx
+++ b/ui/Evaluation Filter/Protokolle.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefan/Documents/Code/Javascript/Getaviz/ui/Evaluation Filter/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{6C2ABADA-7948-004B-9171-0967CEE47DCD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test (David)" sheetId="2" r:id="rId1"/>
@@ -22,6 +23,9 @@
     <sheet name="Teilnehmer 5 (Isabell)" sheetId="8" r:id="rId8"/>
     <sheet name="Teilnehmer 6 (Max)" sheetId="9" r:id="rId9"/>
     <sheet name="Teilnehmer 7 (Johannes)" sheetId="10" r:id="rId10"/>
+    <sheet name="Teilnehmer 8 (Alex)" sheetId="11" r:id="rId11"/>
+    <sheet name="Teilnehmer 9 (Janos)" sheetId="12" r:id="rId12"/>
+    <sheet name="Teilnehmer 10 (Lisa)" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="150000"/>
   <extLst>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="144">
   <si>
     <t>Protokoll RedPill</t>
   </si>
@@ -432,12 +436,48 @@
   </si>
   <si>
     <t>vorgefertigte Konfigurationen gewünscht</t>
+  </si>
+  <si>
+    <t>Uhrzeit: 18:08</t>
+  </si>
+  <si>
+    <t>Containerauswertungsreihenfolge wichtig für's Verständnis</t>
+  </si>
+  <si>
+    <t>nutzt selected transformation statt visibile</t>
+  </si>
+  <si>
+    <t>Uhrzeit: 18:51</t>
+  </si>
+  <si>
+    <t>Uhrzeit: 13:20 Uhr</t>
+  </si>
+  <si>
+    <t>Proband erwartet dass sich Transformationen überlagern (visible und transparent)</t>
+  </si>
+  <si>
+    <t>Will gesamte PhoneUtils Klasse sehen und Beziehungen selected</t>
+  </si>
+  <si>
+    <t>relationen aufteilen in innerhalb &amp; außerhalb</t>
+  </si>
+  <si>
+    <t>Uhrzeit: 14:16 Uhr</t>
+  </si>
+  <si>
+    <t>Uhrzeit: 15:00 Uhr</t>
+  </si>
+  <si>
+    <t>vorschlagseinschränkung verwirrt</t>
+  </si>
+  <si>
+    <t>Uhrzeit: 15:45 Uhr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -497,10 +537,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -853,7 +920,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H39"/>
   <sheetViews>
@@ -868,38 +935,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="D1" s="22" t="s">
+      <c r="B1" s="30"/>
+      <c r="D1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -908,13 +975,13 @@
       <c r="B4" s="2">
         <v>0.54722222222222217</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1114,20 +1181,20 @@
     <mergeCell ref="D4:H4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
-    <hyperlink ref="D1" r:id="rId4"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D1" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -1138,57 +1205,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="D1" s="22" t="s">
+      <c r="B1" s="30"/>
+      <c r="D1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="35"/>
       <c r="D5" s="18"/>
       <c r="E5" s="19"/>
       <c r="F5" s="19"/>
@@ -1212,19 +1279,19 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="33" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="33" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="20" t="s">
@@ -1232,31 +1299,31 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="20" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="24"/>
+      <c r="A12" s="33"/>
       <c r="B12" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
+      <c r="A13" s="33"/>
       <c r="B13" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
+      <c r="A14" s="33"/>
       <c r="B14" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
+      <c r="A15" s="33"/>
       <c r="B15" t="s">
         <v>80</v>
       </c>
@@ -1390,17 +1457,827 @@
     <mergeCell ref="D4:H4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
-    <hyperlink ref="D1" r:id="rId4"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
+    <hyperlink ref="D1" r:id="rId4" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:H34"/>
+  <sheetViews>
+    <sheetView showRuler="0" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="137" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="D1" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D2" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="34"/>
+      <c r="B5" s="35"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="33"/>
+      <c r="B11" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="33"/>
+      <c r="B12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="33"/>
+      <c r="B13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="33"/>
+      <c r="B14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="33"/>
+      <c r="B15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="D4:H4"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0A00-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0A00-000002000000}"/>
+    <hyperlink ref="D1" r:id="rId4" xr:uid="{00000000-0004-0000-0A00-000003000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48FDEAFC-AFBD-DE4F-9E16-4B685A4157B8}">
+  <dimension ref="A1:H34"/>
+  <sheetViews>
+    <sheetView showRuler="0" topLeftCell="A5" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="137" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="D1" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D2" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="34"/>
+      <c r="B5" s="35"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="33"/>
+      <c r="B11" s="26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="33"/>
+      <c r="B12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="33"/>
+      <c r="B13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="33"/>
+      <c r="B14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="33"/>
+      <c r="B15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="D4:H4"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{0555E2F0-6D27-0C44-B626-8DB069E34360}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{9EBF2F02-E99F-4542-B8AA-5028A7A7D4F2}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{11461B47-52EC-304D-A92A-044CD65CFB82}"/>
+    <hyperlink ref="D1" r:id="rId4" xr:uid="{D984533A-D458-9D4F-B393-49828E797C28}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D87A1E65-AA2C-C04A-A7B2-D879B9D17116}">
+  <dimension ref="A1:H34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="137" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="D1" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D2" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="34"/>
+      <c r="B5" s="35"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="33"/>
+      <c r="B11" s="29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="33"/>
+      <c r="B12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="33"/>
+      <c r="B13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="33"/>
+      <c r="B14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="33"/>
+      <c r="B15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="D4:H4"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{94714097-5CC7-8E4F-91F6-4F3B8D3353B7}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{EE5E0C6C-02F8-3345-94C2-6CCD80016CCE}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{61B44C79-12FF-7742-8509-196EACD5E3E1}"/>
+    <hyperlink ref="D1" r:id="rId4" xr:uid="{335D6189-C7E5-6448-B945-B280AF1DE20C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H45"/>
   <sheetViews>
@@ -1415,38 +2292,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="D1" s="22" t="s">
+      <c r="B1" s="30"/>
+      <c r="D1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1455,13 +2332,13 @@
       <c r="B4" s="2">
         <v>0.58819444444444446</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1673,17 +2550,17 @@
     <mergeCell ref="D1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
-    <hyperlink ref="D1" r:id="rId4"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="D1" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
@@ -1700,57 +2577,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="D1" s="22" t="s">
+      <c r="B1" s="30"/>
+      <c r="D1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="35"/>
       <c r="D5" s="3"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -1774,19 +2651,19 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="33" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="33" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1794,31 +2671,31 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="5" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="24"/>
+      <c r="A12" s="33"/>
       <c r="B12" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
+      <c r="A13" s="33"/>
       <c r="B13" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
+      <c r="A14" s="33"/>
       <c r="B14" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
+      <c r="A15" s="33"/>
       <c r="B15" t="s">
         <v>80</v>
       </c>
@@ -1940,17 +2817,17 @@
     <mergeCell ref="B4:B5"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
-    <hyperlink ref="D1" r:id="rId4"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="D1" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
@@ -1967,57 +2844,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="D1" s="22" t="s">
+      <c r="B1" s="30"/>
+      <c r="D1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="35"/>
       <c r="D5" s="6"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
@@ -2041,19 +2918,19 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="33" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="33" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -2061,31 +2938,31 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="8" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="24"/>
+      <c r="A12" s="33"/>
       <c r="B12" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
+      <c r="A13" s="33"/>
       <c r="B13" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
+      <c r="A14" s="33"/>
       <c r="B14" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
+      <c r="A15" s="33"/>
       <c r="B15" t="s">
         <v>80</v>
       </c>
@@ -2244,17 +3121,17 @@
     <mergeCell ref="D4:H4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
-    <hyperlink ref="D1" r:id="rId4"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="D1" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -2268,57 +3145,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="D1" s="22" t="s">
+      <c r="B1" s="30"/>
+      <c r="D1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="35"/>
       <c r="D5" s="9"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
@@ -2342,19 +3219,19 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="33" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="33" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="11" t="s">
@@ -2362,31 +3239,31 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="11" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="24"/>
+      <c r="A12" s="33"/>
       <c r="B12" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
+      <c r="A13" s="33"/>
       <c r="B13" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
+      <c r="A14" s="33"/>
       <c r="B14" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
+      <c r="A15" s="33"/>
       <c r="B15" t="s">
         <v>80</v>
       </c>
@@ -2528,17 +3405,17 @@
     <mergeCell ref="D4:H4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
-    <hyperlink ref="D1" r:id="rId4"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="D1" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -2552,57 +3429,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="D1" s="22" t="s">
+      <c r="B1" s="30"/>
+      <c r="D1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="35"/>
       <c r="D5" s="12"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
@@ -2626,19 +3503,19 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="33" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="33" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="14" t="s">
@@ -2646,31 +3523,31 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="14" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="24"/>
+      <c r="A12" s="33"/>
       <c r="B12" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
+      <c r="A13" s="33"/>
       <c r="B13" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
+      <c r="A14" s="33"/>
       <c r="B14" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
+      <c r="A15" s="33"/>
       <c r="B15" t="s">
         <v>80</v>
       </c>
@@ -2809,17 +3686,17 @@
     <mergeCell ref="D4:H4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
-    <hyperlink ref="D1" r:id="rId4"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="D1" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -2833,57 +3710,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="D1" s="22" t="s">
+      <c r="B1" s="30"/>
+      <c r="D1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="35"/>
       <c r="D5" s="12"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
@@ -2907,19 +3784,19 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="33" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="33" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="14" t="s">
@@ -2927,31 +3804,31 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="14" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="24"/>
+      <c r="A12" s="33"/>
       <c r="B12" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
+      <c r="A13" s="33"/>
       <c r="B13" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
+      <c r="A14" s="33"/>
       <c r="B14" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
+      <c r="A15" s="33"/>
       <c r="B15" t="s">
         <v>80</v>
       </c>
@@ -3084,17 +3961,17 @@
     <mergeCell ref="D4:H4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
-    <hyperlink ref="D1" r:id="rId4"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="D1" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView showRuler="0" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -3108,57 +3985,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="D1" s="22" t="s">
+      <c r="B1" s="30"/>
+      <c r="D1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="35"/>
       <c r="D5" s="15"/>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
@@ -3182,19 +4059,19 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="33" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="33" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="17" t="s">
@@ -3202,31 +4079,31 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="17" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="24"/>
+      <c r="A12" s="33"/>
       <c r="B12" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
+      <c r="A13" s="33"/>
       <c r="B13" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
+      <c r="A14" s="33"/>
       <c r="B14" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
+      <c r="A15" s="33"/>
       <c r="B15" t="s">
         <v>80</v>
       </c>
@@ -3351,17 +4228,17 @@
     <mergeCell ref="D4:H4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
-    <hyperlink ref="D1" r:id="rId4"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
+    <hyperlink ref="D1" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -3375,57 +4252,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="D1" s="22" t="s">
+      <c r="B1" s="30"/>
+      <c r="D1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="35"/>
       <c r="D5" s="18"/>
       <c r="E5" s="19"/>
       <c r="F5" s="19"/>
@@ -3449,19 +4326,19 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="33" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="33" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="20" t="s">
@@ -3469,31 +4346,31 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="20" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="24"/>
+      <c r="A12" s="33"/>
       <c r="B12" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
+      <c r="A13" s="33"/>
       <c r="B13" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
+      <c r="A14" s="33"/>
       <c r="B14" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
+      <c r="A15" s="33"/>
       <c r="B15" t="s">
         <v>80</v>
       </c>
@@ -3624,10 +4501,10 @@
     <mergeCell ref="D4:H4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D2" r:id="rId3"/>
-    <hyperlink ref="D1" r:id="rId4"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="D1" r:id="rId4" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>